<commit_message>
0.0.12: Enable searching telegram object for property.
</commit_message>
<xml_diff>
--- a/meta/api/GetTableSample5.xlsx
+++ b/meta/api/GetTableSample5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7C713C-6941-DE44-80A3-73CF4A878948}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AEA3BF-D7AD-444F-9D37-44E56DD42EEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="460" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="460" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -3466,12 +3466,87 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="59" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3481,9 +3556,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3496,12 +3568,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3540,84 +3606,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3638,12 +3626,27 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3667,9 +3670,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4261,137 +4261,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="184" t="s">
+      <c r="A5" s="138" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="184"/>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="181" t="s">
+      <c r="A6" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="182"/>
-      <c r="C6" s="183"/>
-      <c r="D6" s="180" t="s">
+      <c r="B6" s="143"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="139" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="180"/>
+      <c r="E6" s="139"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="184" t="s">
+      <c r="A7" s="138" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="184"/>
-      <c r="C7" s="184"/>
-      <c r="D7" s="180" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="139" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="180"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="184" t="s">
+      <c r="A8" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="184"/>
-      <c r="C8" s="184"/>
-      <c r="D8" s="180" t="s">
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="139" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="180"/>
+      <c r="E8" s="139"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="184" t="s">
+      <c r="A9" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="184"/>
-      <c r="C9" s="184"/>
-      <c r="D9" s="180" t="s">
+      <c r="B9" s="138"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="139" t="s">
         <v>179</v>
       </c>
-      <c r="E9" s="180"/>
+      <c r="E9" s="139"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="184" t="s">
+      <c r="A10" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="184"/>
-      <c r="C10" s="184"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
+      <c r="B10" s="138"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="184" t="s">
+      <c r="A11" s="138" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="184"/>
-      <c r="C11" s="184"/>
-      <c r="D11" s="180" t="s">
+      <c r="B11" s="138"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="139" t="s">
         <v>178</v>
       </c>
-      <c r="E11" s="180"/>
+      <c r="E11" s="139"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="143" t="s">
+      <c r="A12" s="145" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="143"/>
-      <c r="C12" s="143"/>
-      <c r="D12" s="164" t="s">
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="164"/>
+      <c r="E12" s="140"/>
       <c r="F12" s="95" t="s">
         <v>137</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="143" t="s">
+      <c r="A13" s="145" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="143"/>
-      <c r="C13" s="143"/>
-      <c r="D13" s="164" t="s">
+      <c r="B13" s="145"/>
+      <c r="C13" s="145"/>
+      <c r="D13" s="140" t="s">
         <v>165</v>
       </c>
-      <c r="E13" s="164"/>
+      <c r="E13" s="140"/>
       <c r="F13" s="95" t="s">
         <v>166</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="145" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="143"/>
-      <c r="C14" s="143"/>
-      <c r="D14" s="163"/>
-      <c r="E14" s="164"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="140"/>
       <c r="F14" s="54" t="s">
         <v>156</v>
       </c>
@@ -4399,15 +4399,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="143" t="s">
+      <c r="A15" s="145" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="143"/>
-      <c r="C15" s="143"/>
-      <c r="D15" s="163" t="s">
+      <c r="B15" s="145"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="141" t="s">
         <v>180</v>
       </c>
-      <c r="E15" s="164"/>
+      <c r="E15" s="140"/>
       <c r="F15" s="54" t="s">
         <v>173</v>
       </c>
@@ -4415,13 +4415,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="143" t="s">
+      <c r="A16" s="145" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="143"/>
-      <c r="C16" s="143"/>
-      <c r="D16" s="163"/>
-      <c r="E16" s="164"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="140"/>
       <c r="F16" s="54" t="s">
         <v>172</v>
       </c>
@@ -4429,15 +4429,15 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="143" t="s">
+      <c r="A17" s="145" t="s">
         <v>169</v>
       </c>
-      <c r="B17" s="143"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="163" t="s">
+      <c r="B17" s="145"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="164"/>
+      <c r="E17" s="140"/>
       <c r="F17" s="54" t="s">
         <v>168</v>
       </c>
@@ -4445,19 +4445,19 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="160" t="s">
+      <c r="A18" s="182" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="161"/>
-      <c r="C18" s="162"/>
+      <c r="B18" s="183"/>
+      <c r="C18" s="184"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="144" t="s">
+      <c r="A19" s="168" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="145"/>
-      <c r="C19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="170"/>
       <c r="D19" s="100"/>
       <c r="E19" t="s">
         <v>140</v>
@@ -4475,15 +4475,15 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="179" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="158"/>
-      <c r="C21" s="158"/>
-      <c r="D21" s="158"/>
-      <c r="E21" s="158"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="180"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="180"/>
+      <c r="G21" s="181"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="101" t="s">
@@ -4531,28 +4531,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="156" t="s">
+      <c r="A26" s="178" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="156"/>
-      <c r="C26" s="156"/>
-      <c r="D26" s="156"/>
-      <c r="E26" s="156"/>
-      <c r="F26" s="156"/>
-      <c r="G26" s="156"/>
+      <c r="B26" s="178"/>
+      <c r="C26" s="178"/>
+      <c r="D26" s="178"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="178"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="150" t="s">
+      <c r="B27" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="151"/>
-      <c r="D27" s="151"/>
-      <c r="E27" s="151"/>
-      <c r="F27" s="151"/>
-      <c r="G27" s="152"/>
+      <c r="C27" s="173"/>
+      <c r="D27" s="173"/>
+      <c r="E27" s="173"/>
+      <c r="F27" s="173"/>
+      <c r="G27" s="174"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4563,12 +4563,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="167"/>
+      <c r="B28" s="161"/>
+      <c r="C28" s="161"/>
+      <c r="D28" s="161"/>
+      <c r="E28" s="161"/>
+      <c r="F28" s="161"/>
+      <c r="G28" s="161"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4579,12 +4579,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="168"/>
-      <c r="C29" s="168"/>
-      <c r="D29" s="168"/>
-      <c r="E29" s="168"/>
-      <c r="F29" s="168"/>
-      <c r="G29" s="168"/>
+      <c r="B29" s="157"/>
+      <c r="C29" s="157"/>
+      <c r="D29" s="157"/>
+      <c r="E29" s="157"/>
+      <c r="F29" s="157"/>
+      <c r="G29" s="157"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4595,12 +4595,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="169"/>
-      <c r="D30" s="169"/>
-      <c r="E30" s="169"/>
-      <c r="F30" s="169"/>
-      <c r="G30" s="169"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
+      <c r="G30" s="159"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4613,28 +4613,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="153" t="s">
+      <c r="A32" s="175" t="s">
         <v>149</v>
       </c>
-      <c r="B32" s="154"/>
-      <c r="C32" s="154"/>
-      <c r="D32" s="154"/>
-      <c r="E32" s="154"/>
-      <c r="F32" s="154"/>
-      <c r="G32" s="155"/>
+      <c r="B32" s="176"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="176"/>
+      <c r="F32" s="176"/>
+      <c r="G32" s="177"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="173" t="s">
+      <c r="B33" s="152" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="173"/>
-      <c r="D33" s="173"/>
-      <c r="E33" s="173"/>
-      <c r="F33" s="173"/>
-      <c r="G33" s="173"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="152"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4645,12 +4645,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="116"/>
-      <c r="B34" s="174"/>
-      <c r="C34" s="174"/>
-      <c r="D34" s="174"/>
-      <c r="E34" s="174"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
+      <c r="B34" s="153"/>
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4661,12 +4661,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="175"/>
-      <c r="C35" s="175"/>
-      <c r="D35" s="175"/>
-      <c r="E35" s="175"/>
-      <c r="F35" s="175"/>
-      <c r="G35" s="175"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="154"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4677,12 +4677,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="176"/>
-      <c r="C36" s="176"/>
-      <c r="D36" s="176"/>
-      <c r="E36" s="176"/>
-      <c r="F36" s="176"/>
-      <c r="G36" s="176"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="155"/>
+      <c r="G36" s="155"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4707,28 +4707,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="153" t="s">
+      <c r="A38" s="175" t="s">
         <v>150</v>
       </c>
-      <c r="B38" s="154"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="154"/>
-      <c r="E38" s="154"/>
-      <c r="F38" s="154"/>
-      <c r="G38" s="155"/>
+      <c r="B38" s="176"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="176"/>
+      <c r="E38" s="176"/>
+      <c r="F38" s="176"/>
+      <c r="G38" s="177"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="173" t="s">
+      <c r="B39" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="C39" s="173"/>
-      <c r="D39" s="173"/>
-      <c r="E39" s="173"/>
-      <c r="F39" s="173"/>
-      <c r="G39" s="173"/>
+      <c r="C39" s="152"/>
+      <c r="D39" s="152"/>
+      <c r="E39" s="152"/>
+      <c r="F39" s="152"/>
+      <c r="G39" s="152"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4739,12 +4739,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="174"/>
-      <c r="C40" s="174"/>
-      <c r="D40" s="174"/>
-      <c r="E40" s="174"/>
-      <c r="F40" s="174"/>
-      <c r="G40" s="177"/>
+      <c r="B40" s="153"/>
+      <c r="C40" s="153"/>
+      <c r="D40" s="153"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="153"/>
+      <c r="G40" s="156"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4755,12 +4755,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="168"/>
-      <c r="C41" s="168"/>
-      <c r="D41" s="168"/>
-      <c r="E41" s="168"/>
-      <c r="F41" s="168"/>
-      <c r="G41" s="178"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="157"/>
+      <c r="D41" s="157"/>
+      <c r="E41" s="157"/>
+      <c r="F41" s="157"/>
+      <c r="G41" s="158"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4771,12 +4771,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="169"/>
-      <c r="C42" s="169"/>
-      <c r="D42" s="169"/>
-      <c r="E42" s="169"/>
-      <c r="F42" s="169"/>
-      <c r="G42" s="179"/>
+      <c r="B42" s="159"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="159"/>
+      <c r="E42" s="159"/>
+      <c r="F42" s="159"/>
+      <c r="G42" s="160"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4811,226 +4811,295 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="140" t="s">
+      <c r="A45" s="165" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="147"/>
-      <c r="C45" s="140" t="s">
+      <c r="B45" s="171"/>
+      <c r="C45" s="165" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="141"/>
-      <c r="E45" s="142"/>
+      <c r="D45" s="166"/>
+      <c r="E45" s="167"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="148"/>
-      <c r="B46" s="149"/>
-      <c r="C46" s="148"/>
-      <c r="D46" s="170"/>
-      <c r="E46" s="149"/>
+      <c r="A46" s="162"/>
+      <c r="B46" s="164"/>
+      <c r="C46" s="162"/>
+      <c r="D46" s="163"/>
+      <c r="E46" s="164"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="138"/>
-      <c r="B47" s="139"/>
-      <c r="C47" s="138"/>
-      <c r="D47" s="171"/>
-      <c r="E47" s="139"/>
+      <c r="A47" s="146"/>
+      <c r="B47" s="148"/>
+      <c r="C47" s="146"/>
+      <c r="D47" s="147"/>
+      <c r="E47" s="148"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="138"/>
-      <c r="B48" s="139"/>
-      <c r="C48" s="138"/>
-      <c r="D48" s="171"/>
-      <c r="E48" s="139"/>
+      <c r="A48" s="146"/>
+      <c r="B48" s="148"/>
+      <c r="C48" s="146"/>
+      <c r="D48" s="147"/>
+      <c r="E48" s="148"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="138"/>
-      <c r="B49" s="139"/>
-      <c r="C49" s="138"/>
-      <c r="D49" s="171"/>
-      <c r="E49" s="139"/>
+      <c r="A49" s="146"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="147"/>
+      <c r="E49" s="148"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="138"/>
-      <c r="B50" s="139"/>
-      <c r="C50" s="138"/>
-      <c r="D50" s="171"/>
-      <c r="E50" s="139"/>
+      <c r="A50" s="146"/>
+      <c r="B50" s="148"/>
+      <c r="C50" s="146"/>
+      <c r="D50" s="147"/>
+      <c r="E50" s="148"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="138"/>
-      <c r="B51" s="139"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="171"/>
-      <c r="E51" s="139"/>
+      <c r="A51" s="146"/>
+      <c r="B51" s="148"/>
+      <c r="C51" s="146"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="148"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="138"/>
-      <c r="B52" s="139"/>
-      <c r="C52" s="138"/>
-      <c r="D52" s="171"/>
-      <c r="E52" s="139"/>
+      <c r="A52" s="146"/>
+      <c r="B52" s="148"/>
+      <c r="C52" s="146"/>
+      <c r="D52" s="147"/>
+      <c r="E52" s="148"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="138"/>
-      <c r="B53" s="139"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="171"/>
-      <c r="E53" s="139"/>
+      <c r="A53" s="146"/>
+      <c r="B53" s="148"/>
+      <c r="C53" s="146"/>
+      <c r="D53" s="147"/>
+      <c r="E53" s="148"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="138"/>
-      <c r="B54" s="139"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="171"/>
-      <c r="E54" s="139"/>
+      <c r="A54" s="146"/>
+      <c r="B54" s="148"/>
+      <c r="C54" s="146"/>
+      <c r="D54" s="147"/>
+      <c r="E54" s="148"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="138"/>
-      <c r="B55" s="139"/>
-      <c r="C55" s="138"/>
-      <c r="D55" s="171"/>
-      <c r="E55" s="139"/>
+      <c r="A55" s="146"/>
+      <c r="B55" s="148"/>
+      <c r="C55" s="146"/>
+      <c r="D55" s="147"/>
+      <c r="E55" s="148"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="138"/>
-      <c r="B56" s="139"/>
-      <c r="C56" s="138"/>
-      <c r="D56" s="171"/>
-      <c r="E56" s="139"/>
+      <c r="A56" s="146"/>
+      <c r="B56" s="148"/>
+      <c r="C56" s="146"/>
+      <c r="D56" s="147"/>
+      <c r="E56" s="148"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="138"/>
-      <c r="B57" s="139"/>
-      <c r="C57" s="138"/>
-      <c r="D57" s="171"/>
-      <c r="E57" s="139"/>
+      <c r="A57" s="146"/>
+      <c r="B57" s="148"/>
+      <c r="C57" s="146"/>
+      <c r="D57" s="147"/>
+      <c r="E57" s="148"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="138"/>
-      <c r="B58" s="139"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="171"/>
-      <c r="E58" s="139"/>
+      <c r="A58" s="146"/>
+      <c r="B58" s="148"/>
+      <c r="C58" s="146"/>
+      <c r="D58" s="147"/>
+      <c r="E58" s="148"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="138"/>
-      <c r="B59" s="139"/>
-      <c r="C59" s="138"/>
-      <c r="D59" s="171"/>
-      <c r="E59" s="139"/>
+      <c r="A59" s="146"/>
+      <c r="B59" s="148"/>
+      <c r="C59" s="146"/>
+      <c r="D59" s="147"/>
+      <c r="E59" s="148"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="138"/>
-      <c r="B60" s="139"/>
-      <c r="C60" s="138"/>
-      <c r="D60" s="171"/>
-      <c r="E60" s="139"/>
+      <c r="A60" s="146"/>
+      <c r="B60" s="148"/>
+      <c r="C60" s="146"/>
+      <c r="D60" s="147"/>
+      <c r="E60" s="148"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="138"/>
-      <c r="B61" s="139"/>
-      <c r="C61" s="138"/>
-      <c r="D61" s="171"/>
-      <c r="E61" s="139"/>
+      <c r="A61" s="146"/>
+      <c r="B61" s="148"/>
+      <c r="C61" s="146"/>
+      <c r="D61" s="147"/>
+      <c r="E61" s="148"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="138"/>
-      <c r="B62" s="139"/>
-      <c r="C62" s="138"/>
-      <c r="D62" s="171"/>
-      <c r="E62" s="139"/>
+      <c r="A62" s="146"/>
+      <c r="B62" s="148"/>
+      <c r="C62" s="146"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="148"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="138"/>
-      <c r="B63" s="139"/>
-      <c r="C63" s="138"/>
-      <c r="D63" s="171"/>
-      <c r="E63" s="139"/>
+      <c r="A63" s="146"/>
+      <c r="B63" s="148"/>
+      <c r="C63" s="146"/>
+      <c r="D63" s="147"/>
+      <c r="E63" s="148"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="138"/>
-      <c r="B64" s="139"/>
-      <c r="C64" s="138"/>
-      <c r="D64" s="171"/>
-      <c r="E64" s="139"/>
+      <c r="A64" s="146"/>
+      <c r="B64" s="148"/>
+      <c r="C64" s="146"/>
+      <c r="D64" s="147"/>
+      <c r="E64" s="148"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="138"/>
-      <c r="B65" s="139"/>
-      <c r="C65" s="138"/>
-      <c r="D65" s="171"/>
-      <c r="E65" s="139"/>
+      <c r="A65" s="146"/>
+      <c r="B65" s="148"/>
+      <c r="C65" s="146"/>
+      <c r="D65" s="147"/>
+      <c r="E65" s="148"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="138"/>
-      <c r="B66" s="139"/>
-      <c r="C66" s="138"/>
-      <c r="D66" s="171"/>
-      <c r="E66" s="139"/>
+      <c r="A66" s="146"/>
+      <c r="B66" s="148"/>
+      <c r="C66" s="146"/>
+      <c r="D66" s="147"/>
+      <c r="E66" s="148"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="138"/>
-      <c r="B67" s="139"/>
-      <c r="C67" s="138"/>
-      <c r="D67" s="171"/>
-      <c r="E67" s="139"/>
+      <c r="A67" s="146"/>
+      <c r="B67" s="148"/>
+      <c r="C67" s="146"/>
+      <c r="D67" s="147"/>
+      <c r="E67" s="148"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="138"/>
-      <c r="B68" s="139"/>
-      <c r="C68" s="138"/>
-      <c r="D68" s="171"/>
-      <c r="E68" s="139"/>
+      <c r="A68" s="146"/>
+      <c r="B68" s="148"/>
+      <c r="C68" s="146"/>
+      <c r="D68" s="147"/>
+      <c r="E68" s="148"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="138"/>
-      <c r="B69" s="139"/>
-      <c r="C69" s="138"/>
-      <c r="D69" s="171"/>
-      <c r="E69" s="139"/>
+      <c r="A69" s="146"/>
+      <c r="B69" s="148"/>
+      <c r="C69" s="146"/>
+      <c r="D69" s="147"/>
+      <c r="E69" s="148"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="165"/>
-      <c r="B70" s="166"/>
-      <c r="C70" s="165"/>
-      <c r="D70" s="172"/>
-      <c r="E70" s="166"/>
+      <c r="A70" s="149"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="149"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="151"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
@@ -5047,80 +5116,11 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5155,8 +5155,8 @@
   </sheetPr>
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5361,10 +5361,10 @@
         <v>91</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="180" t="s">
+      <c r="C14" s="139" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="180"/>
+      <c r="D14" s="139"/>
       <c r="E14" s="54"/>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -5378,10 +5378,10 @@
         <v>136</v>
       </c>
       <c r="B15" s="121"/>
-      <c r="C15" s="164" t="s">
+      <c r="C15" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="164"/>
+      <c r="D15" s="140"/>
       <c r="E15" s="95" t="s">
         <v>137</v>
       </c>
@@ -5396,8 +5396,8 @@
         <v>138</v>
       </c>
       <c r="B16" s="121"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="164"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="140"/>
       <c r="E16" s="55" t="s">
         <v>175</v>
       </c>
@@ -5447,15 +5447,15 @@
       <c r="L18"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="156"/>
-      <c r="C19" s="156"/>
-      <c r="D19" s="156"/>
-      <c r="E19" s="156"/>
-      <c r="F19" s="156"/>
-      <c r="G19" s="156"/>
+      <c r="B19" s="178"/>
+      <c r="C19" s="178"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -5465,14 +5465,14 @@
       <c r="A20" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="150" t="s">
+      <c r="B20" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="151"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="152"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="173"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="174"/>
       <c r="H20" s="105"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -5490,12 +5490,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="116"/>
-      <c r="B21" s="167"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
-      <c r="F21" s="167"/>
-      <c r="G21" s="167"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="161"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="161"/>
+      <c r="F21" s="161"/>
+      <c r="G21" s="161"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -5513,12 +5513,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="117"/>
-      <c r="B22" s="168"/>
-      <c r="C22" s="168"/>
-      <c r="D22" s="168"/>
-      <c r="E22" s="168"/>
-      <c r="F22" s="168"/>
-      <c r="G22" s="168"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="157"/>
+      <c r="F22" s="157"/>
+      <c r="G22" s="157"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -5536,12 +5536,12 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="118"/>
-      <c r="B23" s="169"/>
-      <c r="C23" s="169"/>
-      <c r="D23" s="169"/>
-      <c r="E23" s="169"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="169"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="112"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -5561,15 +5561,15 @@
       <c r="L24" s="105"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="153" t="s">
+      <c r="A25" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="B25" s="154"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="154"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="155"/>
+      <c r="B25" s="176"/>
+      <c r="C25" s="176"/>
+      <c r="D25" s="176"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="176"/>
+      <c r="G25" s="177"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
       <c r="K25" s="105"/>
@@ -5579,14 +5579,14 @@
       <c r="A26" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="152" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="173"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="173"/>
-      <c r="F26" s="173"/>
-      <c r="G26" s="173"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="105"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -5604,12 +5604,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="116"/>
-      <c r="B27" s="174"/>
-      <c r="C27" s="174"/>
-      <c r="D27" s="174"/>
-      <c r="E27" s="174"/>
-      <c r="F27" s="174"/>
-      <c r="G27" s="174"/>
+      <c r="B27" s="153"/>
+      <c r="C27" s="153"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
       <c r="H27" s="112"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -5627,12 +5627,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="117"/>
-      <c r="B28" s="175"/>
-      <c r="C28" s="175"/>
-      <c r="D28" s="175"/>
-      <c r="E28" s="175"/>
-      <c r="F28" s="175"/>
-      <c r="G28" s="175"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
       <c r="H28" s="112"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
@@ -5646,12 +5646,12 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="118"/>
-      <c r="B29" s="176"/>
-      <c r="C29" s="176"/>
-      <c r="D29" s="176"/>
-      <c r="E29" s="176"/>
-      <c r="F29" s="176"/>
-      <c r="G29" s="176"/>
+      <c r="B29" s="155"/>
+      <c r="C29" s="155"/>
+      <c r="D29" s="155"/>
+      <c r="E29" s="155"/>
+      <c r="F29" s="155"/>
+      <c r="G29" s="155"/>
       <c r="H29" s="112"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -5690,15 +5690,15 @@
       <c r="T30"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="153" t="s">
+      <c r="A31" s="175" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="154"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="155"/>
+      <c r="B31" s="176"/>
+      <c r="C31" s="176"/>
+      <c r="D31" s="176"/>
+      <c r="E31" s="176"/>
+      <c r="F31" s="176"/>
+      <c r="G31" s="177"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
       <c r="K31" s="112"/>
@@ -5708,14 +5708,14 @@
       <c r="A32" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="173" t="s">
+      <c r="B32" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="173"/>
-      <c r="D32" s="173"/>
-      <c r="E32" s="173"/>
-      <c r="F32" s="173"/>
-      <c r="G32" s="173"/>
+      <c r="C32" s="152"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="152"/>
+      <c r="F32" s="152"/>
+      <c r="G32" s="152"/>
       <c r="H32" s="105"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -5733,12 +5733,12 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="116"/>
-      <c r="B33" s="167"/>
-      <c r="C33" s="167"/>
-      <c r="D33" s="167"/>
-      <c r="E33" s="167"/>
-      <c r="F33" s="167"/>
-      <c r="G33" s="187"/>
+      <c r="B33" s="161"/>
+      <c r="C33" s="161"/>
+      <c r="D33" s="161"/>
+      <c r="E33" s="161"/>
+      <c r="F33" s="161"/>
+      <c r="G33" s="197"/>
       <c r="H33" s="112"/>
       <c r="I33"/>
       <c r="J33"/>
@@ -5756,12 +5756,12 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="117"/>
-      <c r="B34" s="168"/>
-      <c r="C34" s="168"/>
-      <c r="D34" s="168"/>
-      <c r="E34" s="168"/>
-      <c r="F34" s="168"/>
-      <c r="G34" s="178"/>
+      <c r="B34" s="157"/>
+      <c r="C34" s="157"/>
+      <c r="D34" s="157"/>
+      <c r="E34" s="157"/>
+      <c r="F34" s="157"/>
+      <c r="G34" s="158"/>
       <c r="H34" s="112"/>
       <c r="M34" s="112"/>
       <c r="N34" s="112"/>
@@ -5775,12 +5775,12 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="118"/>
-      <c r="B35" s="169"/>
-      <c r="C35" s="169"/>
-      <c r="D35" s="169"/>
-      <c r="E35" s="169"/>
-      <c r="F35" s="169"/>
-      <c r="G35" s="179"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="160"/>
       <c r="H35" s="112"/>
       <c r="M35" s="112"/>
       <c r="N35" s="112"/>
@@ -5844,82 +5844,82 @@
       <c r="Z38" s="39"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="189" t="s">
+      <c r="A39" s="185" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="189" t="s">
+      <c r="B39" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="191" t="s">
+      <c r="C39" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="189" t="s">
+      <c r="D39" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="192" t="s">
+      <c r="E39" s="188" t="s">
         <v>132</v>
       </c>
-      <c r="F39" s="192" t="s">
+      <c r="F39" s="188" t="s">
         <v>138</v>
       </c>
-      <c r="G39" s="189" t="s">
+      <c r="G39" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="189" t="s">
+      <c r="H39" s="185" t="s">
         <v>95</v>
       </c>
-      <c r="I39" s="188" t="s">
+      <c r="I39" s="192" t="s">
         <v>158</v>
       </c>
-      <c r="J39" s="188" t="s">
+      <c r="J39" s="192" t="s">
         <v>159</v>
       </c>
-      <c r="K39" s="188" t="s">
+      <c r="K39" s="192" t="s">
         <v>160</v>
       </c>
-      <c r="L39" s="196" t="s">
+      <c r="L39" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="M39" s="189" t="s">
+      <c r="M39" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="N39" s="189" t="s">
+      <c r="N39" s="185" t="s">
         <v>164</v>
       </c>
-      <c r="O39" s="191" t="s">
+      <c r="O39" s="187" t="s">
         <v>163</v>
       </c>
-      <c r="P39" s="185" t="s">
+      <c r="P39" s="195" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="186"/>
-      <c r="R39" s="185" t="s">
+      <c r="Q39" s="196"/>
+      <c r="R39" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="S39" s="186"/>
+      <c r="S39" s="196"/>
       <c r="T39" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U39" s="189" t="s">
+      <c r="U39" s="185" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="190"/>
-      <c r="B40" s="190"/>
-      <c r="C40" s="190"/>
-      <c r="D40" s="190"/>
-      <c r="E40" s="193"/>
-      <c r="F40" s="194"/>
-      <c r="G40" s="190"/>
-      <c r="H40" s="190"/>
-      <c r="I40" s="188"/>
-      <c r="J40" s="188"/>
-      <c r="K40" s="188"/>
-      <c r="L40" s="197"/>
-      <c r="M40" s="195"/>
-      <c r="N40" s="195"/>
-      <c r="O40" s="195"/>
+      <c r="A40" s="186"/>
+      <c r="B40" s="186"/>
+      <c r="C40" s="186"/>
+      <c r="D40" s="186"/>
+      <c r="E40" s="189"/>
+      <c r="F40" s="190"/>
+      <c r="G40" s="186"/>
+      <c r="H40" s="186"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
+      <c r="K40" s="192"/>
+      <c r="L40" s="194"/>
+      <c r="M40" s="191"/>
+      <c r="N40" s="191"/>
+      <c r="O40" s="191"/>
       <c r="P40" s="29" t="s">
         <v>75</v>
       </c>
@@ -5935,7 +5935,7 @@
       <c r="T40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U40" s="190"/>
+      <c r="U40" s="186"/>
     </row>
     <row r="41" spans="1:26">
       <c r="A41" s="7">
@@ -5948,7 +5948,7 @@
         <v>188</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>93</v>
+        <v>185</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -6502,6 +6502,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="P39:Q39"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="U39:U40"/>
     <mergeCell ref="A39:A40"/>
@@ -6518,26 +6538,6 @@
     <mergeCell ref="L39:L40"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="M39:M40"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="K39:K40"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -6594,7 +6594,7 @@
   </sheetPr>
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -6770,10 +6770,10 @@
         <v>136</v>
       </c>
       <c r="B12" s="121"/>
-      <c r="C12" s="164" t="s">
+      <c r="C12" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="164"/>
+      <c r="D12" s="140"/>
       <c r="E12" s="95" t="s">
         <v>137</v>
       </c>
@@ -6788,8 +6788,8 @@
         <v>138</v>
       </c>
       <c r="B13" s="121"/>
-      <c r="C13" s="164"/>
-      <c r="D13" s="164"/>
+      <c r="C13" s="140"/>
+      <c r="D13" s="140"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="54"/>
@@ -6829,15 +6829,15 @@
       <c r="L15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="156" t="s">
+      <c r="A16" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="156"/>
-      <c r="C16" s="156"/>
-      <c r="D16" s="156"/>
-      <c r="E16" s="156"/>
-      <c r="F16" s="156"/>
-      <c r="G16" s="156"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="178"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -6848,14 +6848,14 @@
       <c r="A17" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="151"/>
-      <c r="D17" s="151"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="152"/>
+      <c r="C17" s="173"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="174"/>
       <c r="H17" s="105"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -6871,12 +6871,12 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="116"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="161"/>
+      <c r="D18" s="161"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="161"/>
       <c r="H18" s="112"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -6891,12 +6891,12 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="117"/>
-      <c r="B19" s="168"/>
-      <c r="C19" s="168"/>
-      <c r="D19" s="168"/>
-      <c r="E19" s="168"/>
-      <c r="F19" s="168"/>
-      <c r="G19" s="168"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
       <c r="H19" s="112"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -6911,12 +6911,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="118"/>
-      <c r="B20" s="169"/>
-      <c r="C20" s="169"/>
-      <c r="D20" s="169"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -6943,15 +6943,15 @@
       <c r="O21" s="112"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="153" t="s">
+      <c r="A22" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="154"/>
-      <c r="C22" s="154"/>
-      <c r="D22" s="154"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="155"/>
+      <c r="B22" s="176"/>
+      <c r="C22" s="176"/>
+      <c r="D22" s="176"/>
+      <c r="E22" s="176"/>
+      <c r="F22" s="176"/>
+      <c r="G22" s="177"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -6964,14 +6964,14 @@
       <c r="A23" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="173" t="s">
+      <c r="B23" s="152" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="173"/>
-      <c r="D23" s="173"/>
-      <c r="E23" s="173"/>
-      <c r="F23" s="173"/>
-      <c r="G23" s="173"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="105"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -6985,12 +6985,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="116"/>
-      <c r="B24" s="174"/>
-      <c r="C24" s="174"/>
-      <c r="D24" s="174"/>
-      <c r="E24" s="174"/>
-      <c r="F24" s="174"/>
-      <c r="G24" s="174"/>
+      <c r="B24" s="153"/>
+      <c r="C24" s="153"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
       <c r="H24" s="112"/>
       <c r="I24" s="105"/>
       <c r="J24" s="105"/>
@@ -7005,12 +7005,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="117"/>
-      <c r="B25" s="175"/>
-      <c r="C25" s="175"/>
-      <c r="D25" s="175"/>
-      <c r="E25" s="175"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="175"/>
+      <c r="B25" s="154"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="154"/>
       <c r="H25" s="112"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
@@ -7025,12 +7025,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="118"/>
-      <c r="B26" s="176"/>
-      <c r="C26" s="176"/>
-      <c r="D26" s="176"/>
-      <c r="E26" s="176"/>
-      <c r="F26" s="176"/>
-      <c r="G26" s="176"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="155"/>
+      <c r="D26" s="155"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="155"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7069,15 +7069,15 @@
       <c r="T27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="153" t="s">
+      <c r="A28" s="175" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="154"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="155"/>
+      <c r="B28" s="176"/>
+      <c r="C28" s="176"/>
+      <c r="D28" s="176"/>
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="177"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
@@ -7086,14 +7086,14 @@
       <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="173" t="s">
+      <c r="B29" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="173"/>
-      <c r="D29" s="173"/>
-      <c r="E29" s="173"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="173"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -7111,12 +7111,12 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="116"/>
-      <c r="B30" s="167"/>
-      <c r="C30" s="167"/>
-      <c r="D30" s="167"/>
-      <c r="E30" s="167"/>
-      <c r="F30" s="167"/>
-      <c r="G30" s="187"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="161"/>
+      <c r="D30" s="161"/>
+      <c r="E30" s="161"/>
+      <c r="F30" s="161"/>
+      <c r="G30" s="197"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -7134,12 +7134,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="117"/>
-      <c r="B31" s="168"/>
-      <c r="C31" s="168"/>
-      <c r="D31" s="168"/>
-      <c r="E31" s="168"/>
-      <c r="F31" s="168"/>
-      <c r="G31" s="178"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="158"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -7154,12 +7154,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="118"/>
-      <c r="B32" s="169"/>
-      <c r="C32" s="169"/>
-      <c r="D32" s="169"/>
-      <c r="E32" s="169"/>
-      <c r="F32" s="169"/>
-      <c r="G32" s="179"/>
+      <c r="B32" s="159"/>
+      <c r="C32" s="159"/>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="160"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7229,84 +7229,84 @@
       <c r="U35" s="58"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1">
-      <c r="A36" s="192" t="s">
+      <c r="A36" s="188" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="192" t="s">
+      <c r="B36" s="188" t="s">
         <v>98</v>
       </c>
       <c r="C36" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="192" t="s">
+      <c r="D36" s="188" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="192" t="s">
+      <c r="E36" s="188" t="s">
         <v>132</v>
       </c>
-      <c r="F36" s="192" t="s">
+      <c r="F36" s="188" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="192" t="s">
+      <c r="G36" s="188" t="s">
         <v>111</v>
       </c>
-      <c r="H36" s="192" t="s">
+      <c r="H36" s="188" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="202" t="s">
+      <c r="I36" s="203" t="s">
         <v>158</v>
       </c>
-      <c r="J36" s="204" t="s">
+      <c r="J36" s="205" t="s">
         <v>159</v>
       </c>
-      <c r="K36" s="204" t="s">
+      <c r="K36" s="205" t="s">
         <v>160</v>
       </c>
-      <c r="L36" s="196" t="s">
+      <c r="L36" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="M36" s="189" t="s">
+      <c r="M36" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="N36" s="189" t="s">
+      <c r="N36" s="185" t="s">
         <v>164</v>
       </c>
-      <c r="O36" s="191" t="s">
+      <c r="O36" s="187" t="s">
         <v>163</v>
       </c>
-      <c r="P36" s="201" t="s">
+      <c r="P36" s="202" t="s">
         <v>101</v>
       </c>
-      <c r="Q36" s="199"/>
-      <c r="R36" s="198" t="s">
+      <c r="Q36" s="200"/>
+      <c r="R36" s="199" t="s">
         <v>102</v>
       </c>
-      <c r="S36" s="199"/>
+      <c r="S36" s="200"/>
       <c r="T36" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="U36" s="192" t="s">
+      <c r="U36" s="188" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15">
-      <c r="A37" s="200"/>
-      <c r="B37" s="200"/>
+      <c r="A37" s="201"/>
+      <c r="B37" s="201"/>
       <c r="C37" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="200"/>
-      <c r="E37" s="194"/>
-      <c r="F37" s="194"/>
-      <c r="G37" s="200"/>
-      <c r="H37" s="200"/>
-      <c r="I37" s="203"/>
-      <c r="J37" s="205"/>
-      <c r="K37" s="205"/>
-      <c r="L37" s="197"/>
-      <c r="M37" s="195"/>
-      <c r="N37" s="195"/>
-      <c r="O37" s="206"/>
+      <c r="D37" s="201"/>
+      <c r="E37" s="190"/>
+      <c r="F37" s="190"/>
+      <c r="G37" s="201"/>
+      <c r="H37" s="201"/>
+      <c r="I37" s="204"/>
+      <c r="J37" s="206"/>
+      <c r="K37" s="206"/>
+      <c r="L37" s="194"/>
+      <c r="M37" s="191"/>
+      <c r="N37" s="191"/>
+      <c r="O37" s="198"/>
       <c r="P37" s="62" t="s">
         <v>105</v>
       </c>
@@ -7322,7 +7322,7 @@
       <c r="T37" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="U37" s="200"/>
+      <c r="U37" s="201"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="64">
@@ -7904,24 +7904,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="M36:M37"/>
     <mergeCell ref="R36:S36"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="B29:G29"/>
@@ -7938,6 +7920,24 @@
     <mergeCell ref="I36:I37"/>
     <mergeCell ref="J36:J37"/>
     <mergeCell ref="K36:K37"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.0.15: Enable JSON file for Input / Expect data.
</commit_message>
<xml_diff>
--- a/meta/api/GetTableSample5.xlsx
+++ b/meta/api/GetTableSample5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AEA3BF-D7AD-444F-9D37-44E56DD42EEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51587C40-5947-1245-88A7-9FCB96C4F6E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="460" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="580" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="197">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2241,6 +2241,30 @@
   </si>
   <si>
     <t>メモ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JSONデータ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>jsonData</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TableSampleOption</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>jsonContainer</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JSONデータコンテナ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JsonContainer</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -5155,7 +5179,7 @@
   </sheetPr>
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -5972,10 +5996,18 @@
       <c r="X41" s="9"/>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="10"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="25"/>
+      <c r="A42" s="10">
+        <v>2</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>193</v>
+      </c>
       <c r="E42" s="25"/>
       <c r="F42" s="25"/>
       <c r="G42" s="85"/>
@@ -6594,8 +6626,8 @@
   </sheetPr>
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7420,10 +7452,18 @@
       <c r="U40" s="71"/>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="64"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="74"/>
+      <c r="A41" s="64">
+        <v>4</v>
+      </c>
+      <c r="B41" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="73" t="s">
+        <v>195</v>
+      </c>
+      <c r="D41" s="74" t="s">
+        <v>196</v>
+      </c>
       <c r="E41" s="74"/>
       <c r="F41" s="74"/>
       <c r="G41" s="93"/>

</xml_diff>